<commit_message>
10/25/18 Updating repo. sc
</commit_message>
<xml_diff>
--- a/cityOfAaron/src/C260_L06_testCases.xlsx
+++ b/cityOfAaron/src/C260_L06_testCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Documents\CIT260\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Documents\CIT260\CIT260GroupRepo\cityOfAaron\cityOfAaron\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF4A0F15-0F58-4A64-854A-A6C2811A7491}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5400989D-E7B0-41F3-8B01-6C79744999B3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{A80968E1-CDF4-41F1-A21A-5EAA4F6B0310}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,10 +490,10 @@
         <v>-5</v>
       </c>
       <c r="D4">
-        <v>16</v>
+        <v>188</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -524,19 +524,19 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="C6">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="D6">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="E6">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="F6">
-        <v>300</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -578,7 +578,7 @@
         <v>-2</v>
       </c>
       <c r="E10">
-        <v>2815</v>
+        <v>2950</v>
       </c>
       <c r="F10">
         <v>2800</v>

</xml_diff>